<commit_message>
Fix pdf generator, import and export excel -tblIdentitasSarana
</commit_message>
<xml_diff>
--- a/public/excel/IdentitasSarana_Example_Import.xlsx
+++ b/public/excel/IdentitasSarana_Example_Import.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26827"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\sapra\public\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8CEA30B-4F6D-432F-97BC-7C4B1DFC2B3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1C463FF-740F-4C57-AE9D-6186F5943DDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>No.</t>
   </si>
@@ -31,7 +31,22 @@
     <t>Sapu</t>
   </si>
   <si>
-    <t>Pel</t>
+    <t>Tipe</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Keterangan</t>
+  </si>
+  <si>
+    <t>Bukan perangkat IT</t>
+  </si>
+  <si>
+    <t>Perangakt IT</t>
+  </si>
+  <si>
+    <t>Router</t>
   </si>
 </sst>
 </file>
@@ -75,16 +90,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </left>
       <right style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </right>
       <top style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -92,19 +107,34 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -410,64 +440,94 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.44140625" style="3" customWidth="1"/>
+    <col min="1" max="1" width="8.44140625" style="1" customWidth="1"/>
     <col min="2" max="2" width="25.6640625" customWidth="1"/>
+    <col min="3" max="3" width="15.77734375" style="9" customWidth="1"/>
+    <col min="5" max="5" width="10.88671875" customWidth="1"/>
+    <col min="6" max="6" width="18.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="4">
+      <c r="C1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="3">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="4">
+      <c r="C2" s="8">
+        <v>0</v>
+      </c>
+      <c r="E2" s="6">
+        <v>0</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="3">
         <v>2</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="8">
+        <v>1</v>
+      </c>
+      <c r="E3" s="6">
+        <v>1</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4"/>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5"/>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6"/>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7"/>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8"/>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9"/>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10"/>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11"/>
     </row>
   </sheetData>

</xml_diff>